<commit_message>
First Responder Kit upgrade
</commit_message>
<xml_diff>
--- a/First-Responder-Kit/sp_AskBrent-CheckID-List.xlsx
+++ b/First-Responder-Kit/sp_AskBrent-CheckID-List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brent/Dropbox (Brent Ozar Unlimited)/Projects/sp_AskBrent/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brent/Dropbox (Brent Ozar Unlimited)/BOU Employees/Products/Download Pack/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>CheckID</t>
   </si>
@@ -194,7 +194,16 @@
     <t>SQL Compilations/sec</t>
   </si>
   <si>
-    <t>sp_AskBrent Check ID List - v16 2015-07-18</t>
+    <t>sp_AskBrent Check ID List - v20 2016-01-01</t>
+  </si>
+  <si>
+    <t>Outdated sp_AskBrent</t>
+  </si>
+  <si>
+    <t>sp_AskBrent is Over 6 Months Old</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/askbrent/</t>
   </si>
 </sst>
 </file>
@@ -646,13 +655,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,6 +1135,23 @@
       </c>
       <c r="E30" s="5" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>27</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1156,6 +1182,7 @@
     <hyperlink ref="E24" r:id="rId21"/>
     <hyperlink ref="E29" r:id="rId22"/>
     <hyperlink ref="E30" r:id="rId23"/>
+    <hyperlink ref="E31" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>